<commit_message>
update contexts, add xxstvarshere
</commit_message>
<xml_diff>
--- a/inst/extdata/cards_constructs.xlsx
+++ b/inst/extdata/cards_constructs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://clymb-my.sharepoint.com/personal/mbosman_clymb_onmicrosoft_com/Documents/Documents/siera/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="283" documentId="11_F25DC773A252ABDACC10489D895C41C25ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5534126-6323-4A98-A3C6-C4625D5FFE80}"/>
+  <xr:revisionPtr revIDLastSave="284" documentId="11_F25DC773A252ABDACC10489D895C41C25ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{461FAB2F-1ED5-417C-A17E-BC4EA8A49D04}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="691" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -129,9 +129,6 @@
     <t>Reference ARS location(s)</t>
   </si>
   <si>
-    <t>Comma-separated list of all Analysis Grouping Variables Variable (no quotes)</t>
-  </si>
-  <si>
     <t>Analysis Grouping Variable (Group 2)</t>
   </si>
   <si>
@@ -1281,6 +1278,9 @@
     ,denominator = denom_dataset
   ) }</t>
     </r>
+  </si>
+  <si>
+    <t>Comma-separated list of all Analysis Grouping Variables (no quotes)</t>
   </si>
 </sst>
 </file>
@@ -1647,10 +1647,10 @@
   <sheetData>
     <row r="2" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1662,8 +1662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1683,7 +1683,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>15</v>
@@ -1692,13 +1692,13 @@
         <v>29</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="72" x14ac:dyDescent="0.3">
@@ -1706,7 +1706,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>16</v>
@@ -1715,13 +1715,13 @@
         <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -1729,7 +1729,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>18</v>
@@ -1738,13 +1738,13 @@
         <v>19</v>
       </c>
       <c r="E3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1752,7 +1752,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>23</v>
@@ -1761,13 +1761,13 @@
         <v>24</v>
       </c>
       <c r="E4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1775,7 +1775,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>25</v>
@@ -1784,13 +1784,13 @@
         <v>26</v>
       </c>
       <c r="E5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1798,7 +1798,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>27</v>
@@ -1807,13 +1807,13 @@
         <v>28</v>
       </c>
       <c r="E6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="230.4" x14ac:dyDescent="0.3">
@@ -1821,22 +1821,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="E7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="72" x14ac:dyDescent="0.3">
@@ -1844,22 +1844,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>30</v>
+        <v>92</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -1867,22 +1867,22 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="E9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="288" x14ac:dyDescent="0.3">
@@ -1890,22 +1890,22 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="E10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
@@ -1913,22 +1913,22 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="E11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -1936,22 +1936,22 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="E12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="72" x14ac:dyDescent="0.3">
@@ -1959,22 +1959,22 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E13" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="230.4" x14ac:dyDescent="0.3">
@@ -1982,7 +1982,7 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>21</v>
@@ -1991,13 +1991,13 @@
         <v>22</v>
       </c>
       <c r="E14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="230.4" x14ac:dyDescent="0.3">
@@ -2005,7 +2005,7 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>20</v>
@@ -2014,13 +2014,13 @@
         <v>22</v>
       </c>
       <c r="E15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates cards_constructs with operationId
</commit_message>
<xml_diff>
--- a/inst/extdata/cards_constructs.xlsx
+++ b/inst/extdata/cards_constructs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://clymb-my.sharepoint.com/personal/mbosman_clymb_onmicrosoft_com/Documents/Documents/siera/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="284" documentId="11_F25DC773A252ABDACC10489D895C41C25ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{461FAB2F-1ED5-417C-A17E-BC4EA8A49D04}"/>
+  <xr:revisionPtr revIDLastSave="300" documentId="11_F25DC773A252ABDACC10489D895C41C25ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C44C6C9A-90B7-4CB2-AE8A-2A420EA32232}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="691" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="99">
   <si>
     <t>ana_var</t>
   </si>
@@ -1281,6 +1281,114 @@
   </si>
   <si>
     <t>Comma-separated list of all Analysis Grouping Variables (no quotes)</t>
+  </si>
+  <si>
+    <t>operation_X</t>
+  </si>
+  <si>
+    <t>X'th operation ID for the AnalysisMethod</t>
+  </si>
+  <si>
+    <t>Analyses$method_id -&gt;  AnalysisMethods$operation_id (X'th operation ID)</t>
+  </si>
+  <si>
+    <t>opidXhere</t>
+  </si>
+  <si>
+    <r>
+      <t>df3_analysisidhere &lt;- df3_analysisidhere|&gt;
+           dplyr::filter(stat_name %in% c('n', 'p')) |&gt;
+           dplyr::mutate(operationid = dplyr::case_when(stat_name == 'n' ~ '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>opid1here</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>',
+                                                                                         stat_name == 'p' ~ '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>opid2here</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>df3_An_02 &lt;- df3_An_02|&gt;
+                    dplyr::filter(stat_name %in% c('n', 'p')) |&gt;
+                    dplyr::mutate(operationid = dplyr::case_when(stat_name == 'n' ~ '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mth_03_01_n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>',
+                                                                                                   stat_name == 'p' ~ '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mth_03_02_%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'))</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1660,10 +1768,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1673,7 +1781,7 @@
     <col min="3" max="3" width="43.21875" style="1" customWidth="1"/>
     <col min="4" max="4" width="50" style="1" customWidth="1"/>
     <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="77.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="81.33203125" customWidth="1"/>
     <col min="7" max="7" width="82.21875" customWidth="1"/>
     <col min="8" max="8" width="92.88671875" customWidth="1"/>
   </cols>
@@ -2023,6 +2131,29 @@
         <v>87</v>
       </c>
     </row>
+    <row r="16" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E16" t="s">
+        <v>96</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add warning and tests for xlsx input sheets missing
</commit_message>
<xml_diff>
--- a/inst/extdata/cards_constructs.xlsx
+++ b/inst/extdata/cards_constructs.xlsx
@@ -1770,8 +1770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>